<commit_message>
modify schema field name for matching 2.0.0
</commit_message>
<xml_diff>
--- a/sparc_me/resources/templates/version_2_0_0/schema.xlsx
+++ b/sparc_me/resources/templates/version_2_0_0/schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoa-my.sharepoint.com/personal/lgao142_uoa_auckland_ac_nz/Documents/Desktop/digital-twin-plateform/sparc-me/sparc_me/resources/templates/version_2_0_0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="13_ncr:1_{C3F3CBDE-C2EB-4AB4-B363-E71F4CF56C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C52EFC0-9CE7-4186-8C78-FC796C8EA6E8}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="13_ncr:1_{C3F3CBDE-C2EB-4AB4-B363-E71F4CF56C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A412540-6B00-41FE-B81B-B13EB1929976}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dataset_description" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="resources" sheetId="10" r:id="rId8"/>
     <sheet name="submission" sheetId="3" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -365,9 +365,6 @@
   </si>
   <si>
     <t>sample id</t>
-  </si>
-  <si>
-    <t>wasDerivedFromSample</t>
   </si>
   <si>
     <t>sample experimental group</t>
@@ -971,6 +968,9 @@
   </si>
   <si>
     <t>additional metadata in json format</t>
+  </si>
+  <si>
+    <t>was Derived From</t>
   </si>
 </sst>
 </file>
@@ -1037,6 +1037,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1345,7 +1349,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1362,7 +1366,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -1379,7 +1383,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1396,7 +1400,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1447,7 +1451,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
@@ -1481,7 +1485,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E10" t="s">
         <v>27</v>
@@ -1515,7 +1519,7 @@
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E12" t="s">
         <v>32</v>
@@ -1566,7 +1570,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E15" t="s">
         <v>40</v>
@@ -1583,7 +1587,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
@@ -1600,7 +1604,7 @@
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
@@ -1634,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E19" t="s">
         <v>49</v>
@@ -1668,7 +1672,7 @@
         <v>7</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E21" t="s">
         <v>54</v>
@@ -1685,7 +1689,7 @@
         <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E22" t="s">
         <v>56</v>
@@ -1702,7 +1706,7 @@
         <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E23" t="s">
         <v>58</v>
@@ -1719,7 +1723,7 @@
         <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1736,7 +1740,7 @@
         <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1791,7 +1795,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E2" t="s">
         <v>63</v>
@@ -1808,7 +1812,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E3" t="s">
         <v>65</v>
@@ -1825,7 +1829,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E4" t="s">
         <v>67</v>
@@ -1842,7 +1846,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5" t="s">
         <v>69</v>
@@ -1859,7 +1863,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E6" t="s">
         <v>71</v>
@@ -1876,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E7" t="s">
         <v>73</v>
@@ -1893,7 +1897,7 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E8" t="s">
         <v>75</v>
@@ -1910,7 +1914,7 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E9" t="s">
         <v>77</v>
@@ -1927,7 +1931,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E10" t="s">
         <v>79</v>
@@ -1988,7 +1992,7 @@
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -2005,7 +2009,7 @@
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E16" t="s">
         <v>87</v>
@@ -2033,7 +2037,7 @@
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E18" t="s">
         <v>90</v>
@@ -2061,7 +2065,7 @@
         <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E20" t="s">
         <v>93</v>
@@ -2078,7 +2082,7 @@
         <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E21" t="s">
         <v>95</v>
@@ -2180,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E94F0A20-E7B3-4D8E-AFE6-0B7E0317ACF6}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2219,7 +2223,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E2" t="s">
         <v>63</v>
@@ -2236,15 +2240,15 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
+        <v>276</v>
+      </c>
+      <c r="E3" t="s">
         <v>277</v>
-      </c>
-      <c r="E3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>289</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2253,10 +2257,10 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E4" t="s">
         <v>279</v>
-      </c>
-      <c r="E4" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -2270,7 +2274,7 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E5" t="s">
         <v>65</v>
@@ -2278,16 +2282,16 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
         <v>108</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>109</v>
       </c>
       <c r="E6" t="s">
         <v>67</v>
@@ -2295,36 +2299,36 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" t="s">
         <v>110</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E7" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" t="s">
         <v>112</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>283</v>
-      </c>
-      <c r="E8" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -2362,7 +2366,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2393,15 +2397,15 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -2412,7 +2416,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -2423,7 +2427,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -2434,7 +2438,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -2519,7 +2523,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -2528,12 +2532,12 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -2542,12 +2546,12 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -2556,12 +2560,12 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -2570,15 +2574,15 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E5" t="s">
         <v>287</v>
-      </c>
-      <c r="E5" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2587,7 +2591,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4621751-FF53-4D2F-95AC-6022247E986F}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2630,75 +2634,75 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
         <v>125</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>126</v>
-      </c>
-      <c r="E2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
         <v>128</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>129</v>
-      </c>
-      <c r="E3" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>131</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
         <v>134</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>135</v>
-      </c>
-      <c r="E5" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -2707,7 +2711,7 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -2715,24 +2719,24 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>139</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>140</v>
-      </c>
-      <c r="E7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2741,7 +2745,7 @@
         <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -2749,24 +2753,24 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
         <v>144</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>145</v>
-      </c>
-      <c r="E9" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
@@ -2775,7 +2779,7 @@
         <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -2783,24 +2787,24 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
         <v>149</v>
       </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>150</v>
-      </c>
-      <c r="E11" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -2809,7 +2813,7 @@
         <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -2817,24 +2821,24 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
         <v>154</v>
       </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>155</v>
-      </c>
       <c r="E13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -2843,7 +2847,7 @@
         <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -2851,24 +2855,24 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
         <v>158</v>
       </c>
-      <c r="B15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>159</v>
-      </c>
-      <c r="E15" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -2877,7 +2881,7 @@
         <v>60</v>
       </c>
       <c r="D16" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E16">
         <v>4</v>
@@ -2885,24 +2889,24 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
         <v>163</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>164</v>
-      </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -2911,7 +2915,7 @@
         <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -2919,24 +2923,24 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
         <v>167</v>
       </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>168</v>
-      </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
@@ -2945,7 +2949,7 @@
         <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -2953,24 +2957,24 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>170</v>
+      </c>
+      <c r="B21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
         <v>171</v>
       </c>
-      <c r="B21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>172</v>
-      </c>
-      <c r="E21" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B22" t="s">
         <v>18</v>
@@ -2979,7 +2983,7 @@
         <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2987,21 +2991,21 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>175</v>
+      </c>
+      <c r="B23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" t="s">
         <v>176</v>
       </c>
-      <c r="B23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>177</v>
-      </c>
-      <c r="D23" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
@@ -3010,7 +3014,7 @@
         <v>60</v>
       </c>
       <c r="D24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E24">
         <v>4</v>
@@ -3018,208 +3022,208 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
         <v>181</v>
       </c>
-      <c r="B25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>182</v>
-      </c>
-      <c r="E25" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>183</v>
+      </c>
+      <c r="B26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
         <v>184</v>
       </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>185</v>
-      </c>
-      <c r="E26" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
         <v>187</v>
       </c>
-      <c r="B27" t="s">
-        <v>18</v>
-      </c>
-      <c r="C27" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>188</v>
-      </c>
-      <c r="E27" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
         <v>190</v>
       </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>191</v>
-      </c>
-      <c r="E28" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>192</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
         <v>193</v>
       </c>
-      <c r="B29" t="s">
-        <v>18</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" t="s">
-        <v>194</v>
-      </c>
       <c r="E29" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>194</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
         <v>195</v>
       </c>
-      <c r="B30" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" t="s">
-        <v>196</v>
-      </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
         <v>197</v>
       </c>
-      <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" t="s">
-        <v>198</v>
-      </c>
       <c r="E31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
         <v>199</v>
       </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>200</v>
-      </c>
-      <c r="E32" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>201</v>
+      </c>
+      <c r="B33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
         <v>202</v>
       </c>
-      <c r="B33" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" t="s">
-        <v>203</v>
-      </c>
       <c r="E33" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>203</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
         <v>204</v>
       </c>
-      <c r="B34" t="s">
-        <v>18</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>205</v>
-      </c>
-      <c r="E34" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
         <v>207</v>
       </c>
-      <c r="B35" t="s">
-        <v>18</v>
-      </c>
-      <c r="C35" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>208</v>
-      </c>
-      <c r="E35" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>209</v>
+      </c>
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" t="s">
+        <v>176</v>
+      </c>
+      <c r="D36" t="s">
         <v>210</v>
-      </c>
-      <c r="B36" t="s">
-        <v>18</v>
-      </c>
-      <c r="C36" t="s">
-        <v>177</v>
-      </c>
-      <c r="D36" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
         <v>18</v>
@@ -3228,7 +3232,7 @@
         <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E37">
         <v>10</v>
@@ -3236,7 +3240,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
         <v>18</v>
@@ -3245,7 +3249,7 @@
         <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -3253,19 +3257,19 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>215</v>
+      </c>
+      <c r="B39" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
         <v>216</v>
       </c>
-      <c r="B39" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" t="s">
-        <v>217</v>
-      </c>
       <c r="E39" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -3312,149 +3316,149 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D2" t="s">
         <v>218</v>
       </c>
-      <c r="D2" t="s">
-        <v>219</v>
-      </c>
       <c r="E2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
         <v>220</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D3" t="s">
-        <v>221</v>
-      </c>
       <c r="E3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
         <v>222</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>218</v>
-      </c>
-      <c r="D4" t="s">
-        <v>223</v>
-      </c>
       <c r="E4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" t="s">
         <v>224</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D5" t="s">
-        <v>225</v>
-      </c>
       <c r="E5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>225</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D6" t="s">
         <v>226</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D6" t="s">
-        <v>227</v>
-      </c>
       <c r="E6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>217</v>
+      </c>
+      <c r="D7" t="s">
         <v>228</v>
       </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>218</v>
-      </c>
-      <c r="D7" t="s">
-        <v>229</v>
-      </c>
       <c r="E7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>217</v>
+      </c>
+      <c r="D8" t="s">
         <v>230</v>
       </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D8" t="s">
-        <v>231</v>
-      </c>
       <c r="E8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" t="s">
         <v>232</v>
       </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D9" t="s">
-        <v>233</v>
-      </c>
       <c r="E9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" t="s">
         <v>234</v>
       </c>
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>218</v>
-      </c>
-      <c r="D10" t="s">
-        <v>235</v>
-      </c>
       <c r="E10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -3507,7 +3511,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -3515,7 +3519,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -3523,7 +3527,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -3531,7 +3535,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -3539,7 +3543,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
@@ -3587,35 +3591,35 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>240</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>242</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>244</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>